<commit_message>
Eliminacion baner index del modelo anterior
</commit_message>
<xml_diff>
--- a/PROGRAMA/backendHappyPockets/src/main/java/com/happyPockets/service/usuarios.xlsx
+++ b/PROGRAMA/backendHappyPockets/src/main/java/com/happyPockets/service/usuarios.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rayan\OneDrive\Escritorio\Ideas ISS\proyecto----iis\backendHappyPockets\src\main\java\com\happyPockets\service\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Equipo\Desktop\proyecto----iis\PROGRAMA\backendHappyPockets\src\main\java\com\happyPockets\service\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2889AD-2562-4F51-B7CA-2F5A2555735E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D618A89-0D4B-4AF6-872B-1F99CC09E023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6900" yWindow="540" windowWidth="21600" windowHeight="11295" xr2:uid="{A5FDF81B-2D84-445F-8552-85FD48BFE141}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A5FDF81B-2D84-445F-8552-85FD48BFE141}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
   <si>
     <t>Username</t>
   </si>
@@ -78,57 +78,6 @@
   </si>
   <si>
     <t>admin@gmail.com</t>
-  </si>
-  <si>
-    <t>testing</t>
-  </si>
-  <si>
-    <t>testing@gmail.com</t>
-  </si>
-  <si>
-    <t>tesing</t>
-  </si>
-  <si>
-    <t>test2</t>
-  </si>
-  <si>
-    <t>test2@gmail.com</t>
-  </si>
-  <si>
-    <t>testeando</t>
-  </si>
-  <si>
-    <t>testeando@gmail.com</t>
-  </si>
-  <si>
-    <t>testi</t>
-  </si>
-  <si>
-    <t>testi@gmail.com</t>
-  </si>
-  <si>
-    <t>ttest</t>
-  </si>
-  <si>
-    <t>tesst@gmail.com</t>
-  </si>
-  <si>
-    <t>tete</t>
-  </si>
-  <si>
-    <t>tete@gmail.com</t>
-  </si>
-  <si>
-    <t>omo</t>
-  </si>
-  <si>
-    <t>omo@gmail.com</t>
-  </si>
-  <si>
-    <t>res</t>
-  </si>
-  <si>
-    <t>res@gmail.com</t>
   </si>
   <si>
     <t>manuel</t>
@@ -141,7 +90,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -518,314 +466,130 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{840CBCE0-B017-42F4-BF81-0430A436564B}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="23.140625"/>
+    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="0">
+      <c r="G2">
         <v>651274927</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="0">
+      <c r="G3">
         <v>612345678</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" t="s" s="0">
+      <c r="F4" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="0">
+      <c r="G4">
         <v>987654321</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="F5" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="G5" t="n" s="0">
-        <v>9.63852741E8</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="F6" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="G6" t="n" s="0">
-        <v>7.41852963E8</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="E7" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="F7" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="G7" t="n" s="0">
-        <v>9.87654321E8</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="D8" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="E8" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="F8" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="G8" t="n" s="0">
-        <v>9.17382645E8</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="B9" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C9" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="D9" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="E9" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="F9" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="G9" t="n" s="0">
-        <v>8.24671395E8</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="B10" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="D10" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="E10" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="F10" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="G10" t="n" s="0">
-        <v>1.23456789E8</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="B11" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="C11" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="D11" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="E11" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="F11" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="G11" t="n" s="0">
-        <v>1.4702589E7</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="B12" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="C12" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="D12" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="E12" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="F12" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="G12" t="n" s="0">
-        <v>1.11222333E8</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="B13" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="C13" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D13" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="E13" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="F13" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="G13" t="n" s="0">
-        <v>2.22333444E8</v>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5">
+        <v>222333444</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
loader eliminado en index
</commit_message>
<xml_diff>
--- a/PROGRAMA/backendHappyPockets/src/main/java/com/happyPockets/service/usuarios.xlsx
+++ b/PROGRAMA/backendHappyPockets/src/main/java/com/happyPockets/service/usuarios.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Equipo\Desktop\proyecto----iis\PROGRAMA\backendHappyPockets\src\main\java\com\happyPockets\service\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="18">
   <si>
     <t>Username</t>
   </si>
@@ -84,12 +84,19 @@
   </si>
   <si>
     <t>manuel@gmail.com</t>
+  </si>
+  <si>
+    <t>hoal</t>
+  </si>
+  <si>
+    <t>hoal@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -466,7 +473,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{840CBCE0-B017-42F4-BF81-0430A436564B}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
@@ -474,122 +481,145 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="0">
         <v>651274927</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="0">
         <v>612345678</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="0">
         <v>987654321</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="0">
         <v>222333444</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="G6" t="n" s="0">
+        <v>5.55999111E8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
eliminacion de usuarios innecesarios
</commit_message>
<xml_diff>
--- a/PROGRAMA/backendHappyPockets/src/main/java/com/happyPockets/service/usuarios.xlsx
+++ b/PROGRAMA/backendHappyPockets/src/main/java/com/happyPockets/service/usuarios.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Equipo\Desktop\proyecto----iis\PROGRAMA\backendHappyPockets\src\main\java\com\happyPockets\service\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\proyecto-IS\PROGRAMA\backendHappyPockets\src\main\java\com\happyPockets\service\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D618A89-0D4B-4AF6-872B-1F99CC09E023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A1063B-F9F5-4B07-B4D2-01B60A73696E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A5FDF81B-2D84-445F-8552-85FD48BFE141}"/>
+    <workbookView xWindow="4044" yWindow="2004" windowWidth="17280" windowHeight="8964" xr2:uid="{A5FDF81B-2D84-445F-8552-85FD48BFE141}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
   <si>
     <t>Username</t>
   </si>
@@ -78,58 +78,12 @@
   </si>
   <si>
     <t>admin@gmail.com</t>
-  </si>
-  <si>
-    <t>manuel</t>
-  </si>
-  <si>
-    <t>manuel@gmail.com</t>
-  </si>
-  <si>
-    <t>hoal</t>
-  </si>
-  <si>
-    <t>hoal@gmail.com</t>
-  </si>
-  <si>
-    <t>prueba324</t>
-  </si>
-  <si>
-    <t>probando</t>
-  </si>
-  <si>
-    <t>prueba4324@gmail.com</t>
-  </si>
-  <si>
-    <t>tuki</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>jorge</t>
-  </si>
-  <si>
-    <t>1234</t>
-  </si>
-  <si>
-    <t>1@gmail.com</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -506,199 +460,107 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{840CBCE0-B017-42F4-BF81-0430A436564B}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="A5" sqref="A5:K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="23.140625"/>
+    <col min="3" max="3" width="23.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s" s="0">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="0">
+      <c r="G2">
         <v>651274927</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s" s="0">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="0">
+      <c r="G3">
         <v>612345678</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s" s="0">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" t="s" s="0">
+      <c r="F4" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="0">
+      <c r="G4">
         <v>987654321</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="F5" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="G5" s="0">
-        <v>222333444</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="F6" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="G6" t="n" s="0">
-        <v>5.55999111E8</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="E7" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="F7" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="G7" t="n" s="0">
-        <v>4.3254543E7</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="D8" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="E8" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="F8" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="G8" t="n" s="0">
-        <v>1.23456789E8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>